<commit_message>
updates BOM to include horizontal connectors instead of vertical ones
</commit_message>
<xml_diff>
--- a/Contactor Driver BOM.xlsx
+++ b/Contactor Driver BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajfor\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajfor\OneDrive\Documents\LHR\Contactor-DriverPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60222CCC-23D7-48A7-BBAA-671551F2915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88896C0C-9696-403A-A9D4-92A76A1C0E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81197A05-AFF6-4C5C-B73B-3CE3CD3BA628}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Component</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>https://www.mouser.com/datasheet/2/307/en-b3sl-1093544.pdf</t>
+  </si>
+  <si>
+    <t>Molex Microfit Connector Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/43645-0200?qs=4XSMV6Twtb2TZ7elJDViLw%3D%3D&amp;gclid=CjwKCAjwpayjBhAnEiwA-7enaz5rrXZ-_uL_IGfOE-nYsLismrqezJIPpDvBGMZQ0Ird-ldIHxlpyhoCJCwQAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/276/3/0436450200_CRIMP_HOUSINGS-2866614.pdf</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -532,7 +544,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +609,7 @@
         <v>0.19</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D63" si="0">C3*B3</f>
+        <f t="shared" ref="D3:D35" si="0">C3*B3</f>
         <v>0.57000000000000006</v>
       </c>
       <c r="E3" t="s">
@@ -654,14 +666,14 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>0.97</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>3.88</v>
+        <v>0.97</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -797,249 +809,135 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="3">
-        <v>0</v>
+        <v>1.17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(D2:D13)</f>
+        <v>18.810000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed error in footprint
</commit_message>
<xml_diff>
--- a/Contactor Driver BOM.xlsx
+++ b/Contactor Driver BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajfor\OneDrive\Documents\LHR\Contactor-DriverPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88896C0C-9696-403A-A9D4-92A76A1C0E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2D4692-54E5-491C-AAD8-53D69333A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81197A05-AFF6-4C5C-B73B-3CE3CD3BA628}"/>
   </bookViews>
@@ -107,15 +107,6 @@
     <t>https://tools.molex.com/pdm_docs/sd/436500415_sd.pdf</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/phoenix-contact/1757048/260382?utm_adgroup=Terminal%20Blocks%20-%20Headers%2C%20Plugs%20and%20Sockets&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Connectors%2C%20Interconnects_NEW&amp;utm_term=&amp;utm_content=Terminal%20Blocks%20-%20Headers%2C%20Plugs%20and%20Sockets&amp;gclid=      CjwKCAjwpayjBhAnEiwA-7enayAMzRxyRAF4t1NK0vnVDN9_Si_uMj9bhIJRE9v5utg2miw0JXi2lRoCGlkQAvD_BwE</t>
-  </si>
-  <si>
-    <t>https://www.phoenixcontact.com/product/pdf/api/v1/MTc1NzA0OA?_realm=us&amp;_locale=en-US&amp;blocks=commercial-data%2Ctechnical-data%2Capprovals%2Cclassifications%2Cenvironmental-compliance-data</t>
-  </si>
-  <si>
-    <t>Phoenix Power Connection</t>
-  </si>
-  <si>
     <t>N Channel NexFET power MOSFET</t>
   </si>
   <si>
@@ -162,6 +153,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Right Angle Guardian Assembly</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/151035-0002?qs=DO9858XCo9xdq6dl3fkEXg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/276/3/1510350002_PCB_HEADERS-2852077.pdf</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
     <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="255.5703125" customWidth="1"/>
-    <col min="6" max="6" width="192" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="166.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>0.19</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D35" si="0">C3*B3</f>
+        <f t="shared" ref="D3:D13" si="0">C3*B3</f>
         <v>0.57000000000000006</v>
       </c>
       <c r="E3" t="s">
@@ -675,7 +675,7 @@
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
@@ -696,7 +696,7 @@
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F7" t="s">
@@ -705,28 +705,28 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>5.24</v>
+        <v>19.940000000000001</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>5.24</v>
+        <v>19.940000000000001</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -739,15 +739,15 @@
         <v>3.5</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -760,15 +760,15 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -781,15 +781,15 @@
         <v>0.3</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -802,15 +802,15 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -822,20 +822,20 @@
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
-      <c r="E13" t="s">
-        <v>39</v>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="3">
         <f>SUM(D2:D13)</f>
-        <v>18.810000000000002</v>
+        <v>33.510000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,9 +990,12 @@
     <hyperlink ref="F2" r:id="rId1" xr:uid="{81CC13E4-3FAB-4074-96C8-1BB101878E78}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{9FB69CE4-FD36-4AA5-B5A9-C1A58C889FFF}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{7E54A957-D4D5-4133-A677-14BA83996970}"/>
-    <hyperlink ref="E8" r:id="rId4" display="https://www.digikey.com/en/products/detail/phoenix-contact/1757048/260382?utm_adgroup=Terminal%20Blocks%20-%20Headers%2C%20Plugs%20and%20Sockets&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Connectors%2C%20Interconnects_NEW&amp;utm_term=&amp;utm_content=Terminal%20Blocks%20-%20Headers%2C%20Plugs%20and%20Sockets&amp;gclid=      CjwKCAjwpayjBhAnEiwA-7enayAMzRxyRAF4t1NK0vnVDN9_Si_uMj9bhIJRE9v5utg2miw0JXi2lRoCGlkQAvD_BwE" xr:uid="{F7FB60BC-F64B-47AF-9096-26BF4AF57AD4}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{2FF5206E-E068-4CAC-800F-1D5E37110383}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{217A0453-F142-44E6-AAC6-89063013C721}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{F532AB4E-60A6-4A04-BA13-2843A1D14B8F}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{B48A8CFD-1D83-4AD9-8DCF-B38D889D2972}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Formats version history better, adds datasheets for all components on schematic, and puts board dimension on user comments layer
</commit_message>
<xml_diff>
--- a/Contactor Driver BOM.xlsx
+++ b/Contactor Driver BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajfor\OneDrive\Documents\LHR\Contactor-DriverPCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6368cbb4c1145e2e/Documents/LHR/Contactor-DriverPCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2D4692-54E5-491C-AAD8-53D69333A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{1C2D4692-54E5-491C-AAD8-53D69333A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4B5AA0A-B900-4669-ACA9-EC50E59068B3}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81197A05-AFF6-4C5C-B73B-3CE3CD3BA628}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{81197A05-AFF6-4C5C-B73B-3CE3CD3BA628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Component</t>
   </si>
@@ -152,9 +152,6 @@
     <t>https://www.mouser.com/datasheet/2/276/3/0436450200_CRIMP_HOUSINGS-2866614.pdf</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Right Angle Guardian Assembly</t>
   </si>
   <si>
@@ -162,6 +159,15 @@
   </si>
   <si>
     <t>https://www.mouser.com/datasheet/2/276/3/1510350002_PCB_HEADERS-2852077.pdf</t>
+  </si>
+  <si>
+    <t>Test Point Keystone 5005 Compact</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/5005/255329?utm_adgroup=Test%20Points&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Test%20and%20Measurement_NEW&amp;utm_term=&amp;utm_content=Test%20Points&amp;gclid=Cj0KCQjw7aqkBhDPARIsAKGa0oKNsfYqA_UF18emaB6Bes2r4GuGECpgvsfPrGyHdqsUNjqpVwxYezwaAu8MEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.keyelco.com/userAssets/file/M65p56.pdf</t>
   </si>
 </sst>
 </file>
@@ -171,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +197,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -226,6 +247,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,7 +567,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,13 +632,13 @@
         <v>0.19</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D13" si="0">C3*B3</f>
+        <f t="shared" ref="D3:D14" si="0">C3*B3</f>
         <v>0.57000000000000006</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -636,7 +659,7 @@
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -657,7 +680,7 @@
       <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -678,7 +701,7 @@
       <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -699,13 +722,13 @@
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -718,10 +741,10 @@
         <v>19.940000000000001</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -741,7 +764,7 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -783,7 +806,7 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -804,7 +827,7 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -825,21 +848,39 @@
       <c r="E13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>38</v>
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.38</v>
       </c>
       <c r="D14" s="3">
-        <f>SUM(D2:D13)</f>
-        <v>33.510000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
+      <c r="C15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3">
+        <f>SUM(D2:D14)</f>
+        <v>35.030000000000008</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
@@ -994,8 +1035,20 @@
     <hyperlink ref="E13" r:id="rId5" xr:uid="{217A0453-F142-44E6-AAC6-89063013C721}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{F532AB4E-60A6-4A04-BA13-2843A1D14B8F}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{B48A8CFD-1D83-4AD9-8DCF-B38D889D2972}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{02B3AAC6-4E7A-4A9B-8B8B-D9F7E781BFD3}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{198A6AFD-C52F-4847-9B78-3394C59F7079}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{A45ECC4E-A358-4B3C-A018-D300D3971D24}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{927DDAD9-0D09-4663-949D-8CC98AFC0554}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{CD254EB9-532E-4B3D-B5B4-F42566ADA0B2}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{810B33E0-31D7-493A-BCC7-E4EF5857DBF6}"/>
+    <hyperlink ref="F8" r:id="rId14" xr:uid="{E7C0936C-D8EB-486B-917F-EE5DFA37AA23}"/>
+    <hyperlink ref="F5" r:id="rId15" xr:uid="{E4145AE5-0DD4-426C-AED6-04B1879A4E00}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{00B13A7E-54A7-48D1-A095-A93A869D22C8}"/>
+    <hyperlink ref="F12" r:id="rId17" xr:uid="{8A1B36B6-BBCB-4467-B735-F80B86140392}"/>
+    <hyperlink ref="E14" r:id="rId18" display="https://www.digikey.com/en/products/detail/keystone-electronics/5005/255329?utm_adgroup=Test%20Points&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Test%20and%20Measurement_NEW&amp;utm_term=&amp;utm_content=Test%20Points&amp;gclid=Cj0KCQjw7aqkBhDPARIsAKGa0oKNsfYqA_UF18emaB6Bes2r4GuGECpgvsfPrGyHdqsUNjqpVwxYezwaAu8MEALw_wcB" xr:uid="{6A182F7B-C617-415C-9B46-329B25F59B3B}"/>
+    <hyperlink ref="F14" r:id="rId19" xr:uid="{4B76F50C-5948-4062-BA41-EB1F80E715CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM, PDFs, and added labels for tps
</commit_message>
<xml_diff>
--- a/Contactor Driver BOM.xlsx
+++ b/Contactor Driver BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6368cbb4c1145e2e/Documents/LHR/Contactor-DriverPCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krets\Documents\DevinPCB\Boards\Contactor-DriverPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{1C2D4692-54E5-491C-AAD8-53D69333A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4B5AA0A-B900-4669-ACA9-EC50E59068B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A7B275-972F-4D58-B909-80D60D37A474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{81197A05-AFF6-4C5C-B73B-3CE3CD3BA628}"/>
+    <workbookView xWindow="11670" yWindow="2510" windowWidth="12360" windowHeight="9970" xr2:uid="{81197A05-AFF6-4C5C-B73B-3CE3CD3BA628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Component</t>
   </si>
@@ -53,121 +53,67 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Vishay-General-Semiconductor/V2F22HM3-H?qs=BJlw7L4Cy78MY7ajCA04cw%3D%3D</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
-    <t>Surface Mount TMBS Rectifier</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/445/150080GS75000-3084983.pdf</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/150080GS75000?qs=2kOmHSv6VfQRoTEZVk1mGA%3D%3D</t>
-  </si>
-  <si>
-    <t>Green LED SMD 0805 2012 Metric</t>
-  </si>
-  <si>
-    <t>1uF SMD Capacitor 0805 2012 Metric (Tentative)</t>
-  </si>
-  <si>
-    <t>MOSFET NTR4003NT1G</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/onsemi/NTR4003NT1G?qs=CBDP9nzV7kme%2Fyh64xROOQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/specsheet/C0805C105K3PACTU</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C105K3PAC7800/3471726?utm_adgroup=Capacitors&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Supplier_KEMET&amp;utm_term=&amp;utm_content=Capacitors&amp;gclid=CjwKCAjwpayjBhAnEiwA-7ena1zeNz8DPyW48G1lkTIiAz3gPJvV3DogKLtShlFJym83JbJDA1w_1BoCcKcQAvD_BwE</t>
-  </si>
-  <si>
-    <t>Molex Microfit 1x02 Vertical</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Molex/43650-0215?qs=AplfTeSvkkDe0NAwMnlPNw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/276/0436500215_PCB_HEADERS-148687.pdf</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/308/1/NTR4003N_D-2319203.pdf</t>
-  </si>
-  <si>
-    <t>Molex Microfit 1x04 Vertical</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0436500415/283463?s=N4IgjCBcoLQBxVAYygMwIYBsDOBTANCAPZQDaIAnAAxUD8ArgC4C2A%2BtkfQE5K4C81KiAC6AX1GEATGRBUALAGYAbAFYacsCpGigA&amp;utm_campaign=buynow&amp;utm_medium=supplier</t>
-  </si>
-  <si>
-    <t>https://tools.molex.com/pdm_docs/sd/436500415_sd.pdf</t>
-  </si>
-  <si>
-    <t>N Channel NexFET power MOSFET</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CSD18511KTT?qs=BZBei1rCqCASa9OuYBoiCQ%3D%3D&amp;gclid=CjwKCAjwpayjBhAnEiwA-7ena06OhSw85metqGE6N55C_nCjs8TyfVanjSiGvCzBC5QJAlP3Xnut1BoCwzEQAvD_BwE</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/csd18511ktt.pdf?HQS=dis-mous-null-mousermode-dsf-pf-null-wwe&amp;ts=1684781212318&amp;ref_url=https%253A%252F%252Fwww.mouser.com%252F</t>
-  </si>
-  <si>
-    <t>Resistor SMD 10k</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Kamaya/RMC20K103FTP?qs=mAH9sUMRCtvOlPzezS1zLQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/210/Kamaya_RMC_automotive_series_8_2022__1_-3032429.pdf</t>
-  </si>
-  <si>
-    <t>Resistor SMD 0</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Vishay-Dale/RCC08050000Z0EA?qs=GedFDFLaBXG1XappxO%252Bnuw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.vishay.com/docs/20066/rcce3.pdf</t>
-  </si>
-  <si>
-    <t>Button Switch</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Omron-Electronics/B3SL-1002P?qs=h8kCHL4kpM7r31L1Z%2F%2FPBA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/307/en-b3sl-1093544.pdf</t>
-  </si>
-  <si>
-    <t>Molex Microfit Connector Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Molex/43645-0200?qs=4XSMV6Twtb2TZ7elJDViLw%3D%3D&amp;gclid=CjwKCAjwpayjBhAnEiwA-7enaz5rrXZ-_uL_IGfOE-nYsLismrqezJIPpDvBGMZQ0Ird-ldIHxlpyhoCJCwQAvD_BwE</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/276/3/0436450200_CRIMP_HOUSINGS-2866614.pdf</t>
-  </si>
-  <si>
-    <t>Right Angle Guardian Assembly</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Molex/151035-0002?qs=DO9858XCo9xdq6dl3fkEXg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/276/3/1510350002_PCB_HEADERS-2852077.pdf</t>
-  </si>
-  <si>
-    <t>Test Point Keystone 5005 Compact</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/keystone-electronics/5005/255329?utm_adgroup=Test%20Points&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Test%20and%20Measurement_NEW&amp;utm_term=&amp;utm_content=Test%20Points&amp;gclid=Cj0KCQjw7aqkBhDPARIsAKGa0oKNsfYqA_UF18emaB6Bes2r4GuGECpgvsfPrGyHdqsUNjqpVwxYezwaAu8MEALw_wcB</t>
-  </si>
-  <si>
-    <t>https://www.keyelco.com/userAssets/file/M65p56.pdf</t>
+    <t>10k Ohm Resistor</t>
+  </si>
+  <si>
+    <t>100k Ohm Resistor</t>
+  </si>
+  <si>
+    <t>10uF Capacitor</t>
+  </si>
+  <si>
+    <t>VSSAF522 Schottky Diode (Flyback)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Vishay-General-Semiconductor/VSSAF522-M3-H?qs=UkDUCjYnTB00gpgD%2Fb%2Fw%252BA%3D%3D&amp;srsltid=AfmBOooAkRChd0P1RtC9IkblNYv2V__zkKRjlSf2cfxi1cnJXTeUqIqe</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Semtech/SD12C.TCT?qs=rBWM4%252BvDhIcn8cYIj7pElQ%3D%3D</t>
+  </si>
+  <si>
+    <t>SD12C.TCT TVS Diode</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>IRLML0030TRPbF Power NMOS</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Infineon-Technologies/IRLML0030TRPBF?qs=9%252BKlkBgLFf0lLJi3xz1alg%3D%3D&amp;srsltid=AfmBOoqvFJKZLoOQ4A-ySpJeYCmdqOT1aAv9ppQv7O4j7Gs3jOODF7jO</t>
+  </si>
+  <si>
+    <t>BZT52-B12-QX 12V Zener Diode</t>
+  </si>
+  <si>
+    <t>Molex Micro-Fit 3.0 2x1 Vertical</t>
+  </si>
+  <si>
+    <t>PMV35EPER Power PMOS</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Nexperia/PMV35EPER?qs=1fQ7IOp4WrhgehyJ3CPNvw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Nexperia/BZT52-B12-QX?qs=rQFj71Wb1eVMbK8ZYprizw%3D%3D&amp;srsltid=AfmBOoo3M714vQmq1Mo82qJrimZYXjLJFCZdt254TmWpOSiuCaGRhsV_</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RT0603FRE0710KL</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TAIYO-YUDEN/TMK212BBJ106MGHT?qs=sGAEpiMZZMsh%252B1woXyUXj6Ion9DcW8uk%2FCsbgn7gICc%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/604-APTD2012LCGCK</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Vishay-Dale/CRCW0805100KFKEAC?qs=sGAEpiMZZMvdGkrng054t0DrEhLhGh8gZRT9GjFuHWDV3jEqj5sSqw%3D%3D</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -244,11 +190,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -268,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -414,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,23 +508,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A34B95-224A-40C0-9297-8EE4C3B5C0A4}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.5703125" customWidth="1"/>
-    <col min="6" max="6" width="166.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.54296875" customWidth="1"/>
+    <col min="6" max="6" width="166.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,458 +541,370 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.73</v>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.1</v>
       </c>
       <c r="D2" s="3">
-        <f>C2*B2</f>
-        <v>1.46</v>
+        <f t="shared" ref="D2:D15" si="0">C2*B2</f>
+        <v>0.1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D14" si="0">C3*B3</f>
-        <v>0.57000000000000006</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
       <c r="B4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>0.4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5*B5</f>
+        <v>1.98</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>12</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>0.97</v>
+        <v>0.9</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>0.97</v>
+        <v>0.9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
-        <v>1.28</v>
+        <v>0.4</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>1.28</v>
+        <v>1.6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
-        <v>19.940000000000001</v>
+        <v>0.39</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>19.940000000000001</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
-        <v>1.75</v>
+        <v>0.54</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.54</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.85</v>
+        <v>11</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.39</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>1.17</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.38</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>1.52</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3">
-        <f>SUM(D2:D14)</f>
-        <v>35.030000000000008</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f>SUM(D2:D10)</f>
+        <v>7.3</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D13" s="3"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D64" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{81CC13E4-3FAB-4074-96C8-1BB101878E78}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{9FB69CE4-FD36-4AA5-B5A9-C1A58C889FFF}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{7E54A957-D4D5-4133-A677-14BA83996970}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{2FF5206E-E068-4CAC-800F-1D5E37110383}"/>
-    <hyperlink ref="E13" r:id="rId5" xr:uid="{217A0453-F142-44E6-AAC6-89063013C721}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{F532AB4E-60A6-4A04-BA13-2843A1D14B8F}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{B48A8CFD-1D83-4AD9-8DCF-B38D889D2972}"/>
-    <hyperlink ref="F11" r:id="rId8" xr:uid="{02B3AAC6-4E7A-4A9B-8B8B-D9F7E781BFD3}"/>
-    <hyperlink ref="F13" r:id="rId9" xr:uid="{198A6AFD-C52F-4847-9B78-3394C59F7079}"/>
-    <hyperlink ref="F6" r:id="rId10" xr:uid="{A45ECC4E-A358-4B3C-A018-D300D3971D24}"/>
-    <hyperlink ref="F7" r:id="rId11" xr:uid="{927DDAD9-0D09-4663-949D-8CC98AFC0554}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{CD254EB9-532E-4B3D-B5B4-F42566ADA0B2}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{810B33E0-31D7-493A-BCC7-E4EF5857DBF6}"/>
-    <hyperlink ref="F8" r:id="rId14" xr:uid="{E7C0936C-D8EB-486B-917F-EE5DFA37AA23}"/>
-    <hyperlink ref="F5" r:id="rId15" xr:uid="{E4145AE5-0DD4-426C-AED6-04B1879A4E00}"/>
-    <hyperlink ref="F9" r:id="rId16" xr:uid="{00B13A7E-54A7-48D1-A095-A93A869D22C8}"/>
-    <hyperlink ref="F12" r:id="rId17" xr:uid="{8A1B36B6-BBCB-4467-B735-F80B86140392}"/>
-    <hyperlink ref="E14" r:id="rId18" display="https://www.digikey.com/en/products/detail/keystone-electronics/5005/255329?utm_adgroup=Test%20Points&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Test%20and%20Measurement_NEW&amp;utm_term=&amp;utm_content=Test%20Points&amp;gclid=Cj0KCQjw7aqkBhDPARIsAKGa0oKNsfYqA_UF18emaB6Bes2r4GuGECpgvsfPrGyHdqsUNjqpVwxYezwaAu8MEALw_wcB" xr:uid="{6A182F7B-C617-415C-9B46-329B25F59B3B}"/>
-    <hyperlink ref="F14" r:id="rId19" xr:uid="{4B76F50C-5948-4062-BA41-EB1F80E715CC}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{5D4A2364-A1D7-4948-BD74-B648EA8F2C88}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{7C4A5E82-7FBE-47E8-BA18-966692EB8014}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{708531E3-48DC-42DF-9E35-FC2706116626}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{9DFA0480-CFCD-4107-AFC0-D6A4417E9FD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>